<commit_message>
reading in base file for participation
</commit_message>
<xml_diff>
--- a/trouble_shooting/summer2024/Master_Participation_Data_Set.xlsx
+++ b/trouble_shooting/summer2024/Master_Participation_Data_Set.xlsx
@@ -14,7 +14,76 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="209">
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Host</t>
+  </si>
+  <si>
+    <t>Start time</t>
+  </si>
+  <si>
+    <t>End time</t>
+  </si>
+  <si>
+    <t>Participants</t>
+  </si>
+  <si>
+    <t>Duration (minutes)</t>
+  </si>
+  <si>
+    <t>Total participant minutes</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Unique viewers</t>
+  </si>
+  <si>
+    <t>Max concurrent views</t>
+  </si>
+  <si>
+    <t>Creation time</t>
+  </si>
+  <si>
+    <t>Name (original name)</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Join time</t>
+  </si>
+  <si>
+    <t>Leave time</t>
+  </si>
+  <si>
+    <t>Duration (minutes).1</t>
+  </si>
+  <si>
+    <t>Guest</t>
+  </si>
+  <si>
+    <t>Recording disclaimer response</t>
+  </si>
+  <si>
+    <t>In waiting room</t>
+  </si>
   <si>
     <t>Tai Chi: Full Form Practice M/W/F 3pm ET Summer 2024</t>
   </si>
@@ -34,559 +103,544 @@
     <t>07/15/2024 04:28:49 PM</t>
   </si>
   <si>
-    <t>48</t>
-  </si>
-  <si>
-    <t>115</t>
-  </si>
-  <si>
-    <t>2146</t>
-  </si>
-  <si>
-    <t>Unnamed: 9</t>
-  </si>
-  <si>
-    <t>Unnamed: 10</t>
-  </si>
-  <si>
     <t>Zoom</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
-    <t>-.1</t>
-  </si>
-  <si>
     <t>06/14/2024 11:57:23 AM</t>
   </si>
   <si>
+    <t>SBM Tech Support ( SBM Falls Prevention )</t>
+  </si>
+  <si>
     <t>Woody Fischer</t>
   </si>
   <si>
+    <t>Wayne Snell</t>
+  </si>
+  <si>
+    <t>Brianne Norton</t>
+  </si>
+  <si>
+    <t>Gail Braverman</t>
+  </si>
+  <si>
+    <t>Maurice Dickstein</t>
+  </si>
+  <si>
+    <t>Donna Barnard</t>
+  </si>
+  <si>
+    <t>Eileen Rosenzweig</t>
+  </si>
+  <si>
+    <t>Jan Clarke</t>
+  </si>
+  <si>
+    <t>Robbin Schwartz</t>
+  </si>
+  <si>
+    <t>Charlene Gunsel</t>
+  </si>
+  <si>
+    <t>Natalie Nazarenko</t>
+  </si>
+  <si>
+    <t>Eleanor Avni</t>
+  </si>
+  <si>
+    <t>Maureen Brennan</t>
+  </si>
+  <si>
+    <t>Michael J Pinker</t>
+  </si>
+  <si>
+    <t>Jonathan Miller</t>
+  </si>
+  <si>
+    <t>Lorraine Robinson</t>
+  </si>
+  <si>
+    <t>Christina Montes</t>
+  </si>
+  <si>
+    <t>Gracie Matos</t>
+  </si>
+  <si>
+    <t>Mary Garrison-Dennis</t>
+  </si>
+  <si>
+    <t>Marianne Finn</t>
+  </si>
+  <si>
+    <t>Patricia Howley</t>
+  </si>
+  <si>
+    <t>Fu-Mei Huang</t>
+  </si>
+  <si>
+    <t>Michele Szydlo</t>
+  </si>
+  <si>
+    <t>Beverly Gorham</t>
+  </si>
+  <si>
+    <t>Eileen Tellefsen</t>
+  </si>
+  <si>
+    <t>Bernard Dillon</t>
+  </si>
+  <si>
+    <t>Gail Hoag</t>
+  </si>
+  <si>
+    <t>Marlies Schmidt</t>
+  </si>
+  <si>
+    <t>Carolyn Trunca</t>
+  </si>
+  <si>
+    <t>jennifer pohl</t>
+  </si>
+  <si>
+    <t>Susan Ricercato</t>
+  </si>
+  <si>
+    <t>Elizabeth Chu</t>
+  </si>
+  <si>
+    <t>Josie Howlett</t>
+  </si>
+  <si>
+    <t>Antonio Chu</t>
+  </si>
+  <si>
+    <t>Olivia Huang</t>
+  </si>
+  <si>
+    <t>Kathleen Pearsall</t>
+  </si>
+  <si>
+    <t>Myron Silverman</t>
+  </si>
+  <si>
+    <t>Donna Donahue</t>
+  </si>
+  <si>
+    <t>Rose Micene</t>
+  </si>
+  <si>
+    <t>Carola Borries</t>
+  </si>
+  <si>
+    <t>Toni Crespo</t>
+  </si>
+  <si>
+    <t>Karen Tartick</t>
+  </si>
+  <si>
+    <t>lisa serbin</t>
+  </si>
+  <si>
+    <t>Stuart Rothstein</t>
+  </si>
+  <si>
+    <t>brittany.gambini@stonybrookmedicine.edu</t>
+  </si>
+  <si>
     <t>ruderer@aol.com</t>
   </si>
   <si>
+    <t>waynes6117@gmail.com</t>
+  </si>
+  <si>
+    <t>bln26@yahoo.com</t>
+  </si>
+  <si>
+    <t>gbrave1@optonline.net</t>
+  </si>
+  <si>
+    <t>mauriced@optonline.net</t>
+  </si>
+  <si>
+    <t>cubbinator@gmail.com</t>
+  </si>
+  <si>
+    <t>eileenr1104@yahoo.com</t>
+  </si>
+  <si>
+    <t>jacee915@gmail.com</t>
+  </si>
+  <si>
+    <t>rtwobees@earthlink.net</t>
+  </si>
+  <si>
+    <t>cagunsel@aol.com</t>
+  </si>
+  <si>
+    <t>natnaz@aol.com</t>
+  </si>
+  <si>
+    <t>elliavni@gmail.com</t>
+  </si>
+  <si>
+    <t>maureenjbrennan@gmail.com</t>
+  </si>
+  <si>
+    <t>bluesomec@yahoo.com</t>
+  </si>
+  <si>
+    <t>millerjlm@sbcglobal.net</t>
+  </si>
+  <si>
+    <t>lrobrn@gmail.com</t>
+  </si>
+  <si>
+    <t>christina.montes-malanik@us.nestle.com</t>
+  </si>
+  <si>
+    <t>grm25@optonline.net</t>
+  </si>
+  <si>
+    <t>megd758@gmail.com</t>
+  </si>
+  <si>
+    <t>eleanor177@aol.com</t>
+  </si>
+  <si>
+    <t>phowley@optonline.net</t>
+  </si>
+  <si>
+    <t>shihfumei39@gmail.com</t>
+  </si>
+  <si>
+    <t>michele.szydlo@gmail.com</t>
+  </si>
+  <si>
+    <t>bjgor46@aol.com</t>
+  </si>
+  <si>
+    <t>emae24@aol.com</t>
+  </si>
+  <si>
+    <t>bjdillon1@verizon.net</t>
+  </si>
+  <si>
+    <t>gailshoag@gmail.com</t>
+  </si>
+  <si>
+    <t>marliesschmidt2000@yahoo.com</t>
+  </si>
+  <si>
+    <t>ctrunca@gmail.com</t>
+  </si>
+  <si>
+    <t>jpohlreads@gmail.com</t>
+  </si>
+  <si>
+    <t>susan.ricercato@gmail.com</t>
+  </si>
+  <si>
+    <t>elizabethychu@gmail.com</t>
+  </si>
+  <si>
+    <t>jlovept@twcny.rr.com</t>
+  </si>
+  <si>
+    <t>daylilyton@aol.com</t>
+  </si>
+  <si>
+    <t>mhgarden88@hotmail.com</t>
+  </si>
+  <si>
+    <t>kpearsal@twcny.rr.com</t>
+  </si>
+  <si>
+    <t>mysbny@aol.com</t>
+  </si>
+  <si>
+    <t>geodon65@yahoo.com</t>
+  </si>
+  <si>
+    <t>tor2024rk@gmail.com</t>
+  </si>
+  <si>
+    <t>carola_borries@yahoo.com</t>
+  </si>
+  <si>
+    <t>justtonis2@gmail.com</t>
+  </si>
+  <si>
+    <t>ktartick@gmail.com</t>
+  </si>
+  <si>
+    <t>lisa.serbin@gmail.com</t>
+  </si>
+  <si>
+    <t>rothstein@sympatico.ca</t>
+  </si>
+  <si>
     <t>07/15/2024 02:50:02 PM</t>
   </si>
   <si>
+    <t>07/15/2024 02:51:47 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 02:53:12 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 02:53:13 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 02:55:32 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 02:55:41 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 02:56:04 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 02:56:11 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 02:57:01 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 02:57:05 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 02:57:35 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 02:57:36 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 02:57:40 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 02:57:43 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 02:57:56 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 02:58:35 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 02:59:16 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 02:59:23 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 02:59:42 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 02:59:48 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:00:14 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:00:40 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:00:43 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:01:06 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:01:11 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:03:00 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:03:39 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:03:42 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:04:18 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:05:13 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:05:54 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:05:55 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:05:56 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:06:03 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:07:23 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:07:25 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:08:20 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:10:45 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:15:03 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:28:48 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:29:53 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:30:58 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:51:22 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 04:00:59 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 02:59:39 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:02:16 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 04:28:50 PM</t>
+  </si>
+  <si>
     <t>07/15/2024 03:57:28 PM</t>
   </si>
   <si>
-    <t>68</t>
+    <t>07/15/2024 03:57:14 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 04:28:40 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:58:29 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:29:50 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:55:46 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:37:28 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 04:28:34 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:30:03 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:57:29 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 04:28:35 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:29:46 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 04:28:45 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:30:36 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:59:04 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:29:49 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:29:42 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:23:12 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:35:17 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:57:23 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:29:54 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:47:14 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:23:36 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:57:26 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:23:03 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:29:59 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:29:56 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:23:08 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:57:15 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:31:34 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:57:16 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:29:51 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 04:28:47 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:47:25 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:53:54 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:51:12 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 03:57:27 PM</t>
+  </si>
+  <si>
+    <t>07/15/2024 04:21:39 PM</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>Unnamed: 21</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Wayne Snell</t>
-  </si>
-  <si>
-    <t>Brianne Norton</t>
-  </si>
-  <si>
-    <t>Gail Braverman</t>
-  </si>
-  <si>
-    <t>Maurice Dickstein</t>
-  </si>
-  <si>
-    <t>Donna Barnard</t>
-  </si>
-  <si>
-    <t>Eileen Rosenzweig</t>
-  </si>
-  <si>
-    <t>Jan Clarke</t>
-  </si>
-  <si>
-    <t>Robbin Schwartz</t>
-  </si>
-  <si>
-    <t>Charlene Gunsel</t>
-  </si>
-  <si>
-    <t>Natalie Nazarenko</t>
-  </si>
-  <si>
-    <t>Eleanor Avni</t>
-  </si>
-  <si>
-    <t>Maureen Brennan</t>
-  </si>
-  <si>
-    <t>Michael J Pinker</t>
-  </si>
-  <si>
-    <t>Jonathan Miller</t>
-  </si>
-  <si>
-    <t>Lorraine Robinson</t>
-  </si>
-  <si>
-    <t>Christina Montes</t>
-  </si>
-  <si>
-    <t>Gracie Matos</t>
-  </si>
-  <si>
-    <t>Mary Garrison-Dennis</t>
-  </si>
-  <si>
-    <t>Marianne Finn</t>
-  </si>
-  <si>
-    <t>Patricia Howley</t>
-  </si>
-  <si>
-    <t>Fu-Mei Huang</t>
-  </si>
-  <si>
-    <t>Michele Szydlo</t>
-  </si>
-  <si>
-    <t>Beverly Gorham</t>
-  </si>
-  <si>
-    <t>Eileen Tellefsen</t>
-  </si>
-  <si>
-    <t>Bernard Dillon</t>
-  </si>
-  <si>
-    <t>Gail Hoag</t>
-  </si>
-  <si>
-    <t>Marlies Schmidt</t>
-  </si>
-  <si>
-    <t>Carolyn Trunca</t>
-  </si>
-  <si>
-    <t>jennifer pohl</t>
-  </si>
-  <si>
-    <t>Susan Ricercato</t>
-  </si>
-  <si>
-    <t>Elizabeth Chu</t>
-  </si>
-  <si>
-    <t>Josie Howlett</t>
-  </si>
-  <si>
-    <t>Antonio Chu</t>
-  </si>
-  <si>
-    <t>Olivia Huang</t>
-  </si>
-  <si>
-    <t>Kathleen Pearsall</t>
-  </si>
-  <si>
-    <t>Myron Silverman</t>
-  </si>
-  <si>
-    <t>Donna Donahue</t>
-  </si>
-  <si>
-    <t>Rose Micene</t>
-  </si>
-  <si>
-    <t>Carola Borries</t>
-  </si>
-  <si>
-    <t>Toni Crespo</t>
-  </si>
-  <si>
-    <t>Karen Tartick</t>
-  </si>
-  <si>
-    <t>lisa serbin</t>
-  </si>
-  <si>
-    <t>Stuart Rothstein</t>
-  </si>
-  <si>
-    <t>waynes6117@gmail.com</t>
-  </si>
-  <si>
-    <t>bln26@yahoo.com</t>
-  </si>
-  <si>
-    <t>gbrave1@optonline.net</t>
-  </si>
-  <si>
-    <t>mauriced@optonline.net</t>
-  </si>
-  <si>
-    <t>cubbinator@gmail.com</t>
-  </si>
-  <si>
-    <t>eileenr1104@yahoo.com</t>
-  </si>
-  <si>
-    <t>jacee915@gmail.com</t>
-  </si>
-  <si>
-    <t>rtwobees@earthlink.net</t>
-  </si>
-  <si>
-    <t>cagunsel@aol.com</t>
-  </si>
-  <si>
-    <t>natnaz@aol.com</t>
-  </si>
-  <si>
-    <t>elliavni@gmail.com</t>
-  </si>
-  <si>
-    <t>maureenjbrennan@gmail.com</t>
-  </si>
-  <si>
-    <t>bluesomec@yahoo.com</t>
-  </si>
-  <si>
-    <t>millerjlm@sbcglobal.net</t>
-  </si>
-  <si>
-    <t>lrobrn@gmail.com</t>
-  </si>
-  <si>
-    <t>christina.montes-malanik@us.nestle.com</t>
-  </si>
-  <si>
-    <t>grm25@optonline.net</t>
-  </si>
-  <si>
-    <t>megd758@gmail.com</t>
-  </si>
-  <si>
-    <t>eleanor177@aol.com</t>
-  </si>
-  <si>
-    <t>phowley@optonline.net</t>
-  </si>
-  <si>
-    <t>shihfumei39@gmail.com</t>
-  </si>
-  <si>
-    <t>michele.szydlo@gmail.com</t>
-  </si>
-  <si>
-    <t>bjgor46@aol.com</t>
-  </si>
-  <si>
-    <t>emae24@aol.com</t>
-  </si>
-  <si>
-    <t>bjdillon1@verizon.net</t>
-  </si>
-  <si>
-    <t>gailshoag@gmail.com</t>
-  </si>
-  <si>
-    <t>marliesschmidt2000@yahoo.com</t>
-  </si>
-  <si>
-    <t>ctrunca@gmail.com</t>
-  </si>
-  <si>
-    <t>jpohlreads@gmail.com</t>
-  </si>
-  <si>
-    <t>susan.ricercato@gmail.com</t>
-  </si>
-  <si>
-    <t>elizabethychu@gmail.com</t>
-  </si>
-  <si>
-    <t>jlovept@twcny.rr.com</t>
-  </si>
-  <si>
-    <t>daylilyton@aol.com</t>
-  </si>
-  <si>
-    <t>mhgarden88@hotmail.com</t>
-  </si>
-  <si>
-    <t>kpearsal@twcny.rr.com</t>
-  </si>
-  <si>
-    <t>mysbny@aol.com</t>
-  </si>
-  <si>
-    <t>geodon65@yahoo.com</t>
-  </si>
-  <si>
-    <t>tor2024rk@gmail.com</t>
-  </si>
-  <si>
-    <t>carola_borries@yahoo.com</t>
-  </si>
-  <si>
-    <t>justtonis2@gmail.com</t>
-  </si>
-  <si>
-    <t>ktartick@gmail.com</t>
-  </si>
-  <si>
-    <t>lisa.serbin@gmail.com</t>
-  </si>
-  <si>
-    <t>rothstein@sympatico.ca</t>
-  </si>
-  <si>
-    <t>07/15/2024 02:51:47 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 02:53:12 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 02:53:13 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 02:55:32 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 02:55:41 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 02:56:04 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 02:56:11 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 02:57:01 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 02:57:05 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 02:57:35 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 02:57:36 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 02:57:40 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 02:57:43 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 02:57:56 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 02:58:35 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 02:59:16 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 02:59:23 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 02:59:42 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 02:59:48 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:00:14 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:00:40 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:00:43 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:01:06 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:01:11 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:03:00 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:03:39 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:03:42 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:04:18 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:05:13 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:05:54 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:05:55 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:05:56 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:06:03 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:07:23 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:07:25 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:08:20 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:10:45 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:15:03 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:28:48 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:29:53 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:30:58 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:51:22 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 04:00:59 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 02:59:39 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:02:16 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:57:14 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 04:28:40 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:58:29 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:29:50 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:55:46 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:37:28 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 04:28:34 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:30:03 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:57:29 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 04:28:35 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:29:46 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 04:28:45 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:30:36 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:59:04 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:29:49 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:29:42 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:23:12 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:35:17 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:57:23 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:29:54 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:47:14 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:23:36 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:57:26 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:23:03 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:29:59 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:29:56 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:23:08 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:57:15 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:31:34 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:57:16 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:29:51 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 04:28:47 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:47:25 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:53:54 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:51:12 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 03:57:27 PM</t>
-  </si>
-  <si>
-    <t>07/15/2024 04:21:39 PM</t>
   </si>
 </sst>
 </file>
@@ -944,7 +998,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W47"/>
+  <dimension ref="A1:W49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1023,22 +1077,22 @@
     </row>
     <row r="2" spans="1:23">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G2">
         <v>48</v>
@@ -1050,57 +1104,57 @@
         <v>2146</v>
       </c>
       <c r="L2" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M2" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N2" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O2" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P2" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="Q2" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="R2" t="s">
-        <v>109</v>
+        <v>27</v>
       </c>
       <c r="S2" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="T2">
-        <v>66</v>
+        <v>115</v>
       </c>
       <c r="U2" t="s">
-        <v>20</v>
+        <v>207</v>
       </c>
       <c r="W2" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:23">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G3">
         <v>48</v>
@@ -1112,57 +1166,57 @@
         <v>2146</v>
       </c>
       <c r="L3" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M3" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N3" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O3" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P3" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="Q3" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="R3" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="S3" t="s">
-        <v>5</v>
+        <v>169</v>
       </c>
       <c r="T3">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="U3" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W3" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:23">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G4">
         <v>48</v>
@@ -1174,57 +1228,57 @@
         <v>2146</v>
       </c>
       <c r="L4" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M4" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N4" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O4" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="Q4" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="R4" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="S4" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="T4">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="U4" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W4" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:23">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G5">
         <v>48</v>
@@ -1236,57 +1290,57 @@
         <v>2146</v>
       </c>
       <c r="L5" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M5" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N5" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O5" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P5" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="Q5" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="R5" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="S5" t="s">
-        <v>156</v>
+        <v>28</v>
       </c>
       <c r="T5">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="U5" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W5" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:23">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G6">
         <v>48</v>
@@ -1298,57 +1352,57 @@
         <v>2146</v>
       </c>
       <c r="L6" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M6" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N6" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O6" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P6" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="Q6" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="R6" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="S6" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="T6">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="U6" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W6" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:23">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F7" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G7">
         <v>48</v>
@@ -1360,57 +1414,57 @@
         <v>2146</v>
       </c>
       <c r="L7" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M7" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N7" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O7" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P7" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="Q7" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="R7" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="S7" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="T7">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="U7" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W7" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:23">
       <c r="A8" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F8" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G8">
         <v>48</v>
@@ -1422,57 +1476,57 @@
         <v>2146</v>
       </c>
       <c r="L8" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M8" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N8" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O8" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P8" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="Q8" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="R8" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="S8" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="T8">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="U8" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W8" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:23">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F9" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G9">
         <v>48</v>
@@ -1484,57 +1538,57 @@
         <v>2146</v>
       </c>
       <c r="L9" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M9" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N9" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O9" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P9" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="Q9" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="R9" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="S9" t="s">
-        <v>160</v>
+        <v>174</v>
       </c>
       <c r="T9">
-        <v>92</v>
+        <v>60</v>
       </c>
       <c r="U9" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W9" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:23">
       <c r="A10" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F10" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G10">
         <v>48</v>
@@ -1546,57 +1600,57 @@
         <v>2146</v>
       </c>
       <c r="L10" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M10" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N10" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O10" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P10" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="Q10" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="R10" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="S10" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="T10">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="U10" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W10" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:23">
       <c r="A11" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E11" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F11" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G11">
         <v>48</v>
@@ -1608,57 +1662,57 @@
         <v>2146</v>
       </c>
       <c r="L11" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M11" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N11" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O11" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P11" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="Q11" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="R11" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="S11" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="T11">
-        <v>60</v>
+        <v>92</v>
       </c>
       <c r="U11" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W11" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:23">
       <c r="A12" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E12" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F12" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G12">
         <v>48</v>
@@ -1670,57 +1724,57 @@
         <v>2146</v>
       </c>
       <c r="L12" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M12" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N12" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O12" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P12" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="Q12" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="R12" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="S12" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="T12">
         <v>33</v>
       </c>
       <c r="U12" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W12" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13" spans="1:23">
       <c r="A13" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F13" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G13">
         <v>48</v>
@@ -1732,57 +1786,57 @@
         <v>2146</v>
       </c>
       <c r="L13" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M13" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N13" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O13" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P13" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="Q13" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="R13" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="S13" t="s">
-        <v>163</v>
+        <v>178</v>
       </c>
       <c r="T13">
-        <v>91</v>
+        <v>60</v>
       </c>
       <c r="U13" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W13" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14" spans="1:23">
       <c r="A14" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F14" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G14">
         <v>48</v>
@@ -1794,57 +1848,57 @@
         <v>2146</v>
       </c>
       <c r="L14" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M14" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N14" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O14" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P14" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="Q14" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="R14" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="S14" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="T14">
         <v>33</v>
       </c>
       <c r="U14" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W14" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15" spans="1:23">
       <c r="A15" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E15" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F15" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G15">
         <v>48</v>
@@ -1856,57 +1910,57 @@
         <v>2146</v>
       </c>
       <c r="L15" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M15" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N15" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O15" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P15" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="Q15" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="R15" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="S15" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="T15">
         <v>91</v>
       </c>
       <c r="U15" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W15" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:23">
       <c r="A16" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E16" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F16" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G16">
         <v>48</v>
@@ -1918,57 +1972,57 @@
         <v>2146</v>
       </c>
       <c r="L16" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M16" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N16" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O16" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P16" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="Q16" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="R16" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="S16" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="T16">
         <v>33</v>
       </c>
       <c r="U16" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W16" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="17" spans="1:23">
       <c r="A17" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E17" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F17" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G17">
         <v>48</v>
@@ -1980,57 +2034,57 @@
         <v>2146</v>
       </c>
       <c r="L17" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M17" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N17" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O17" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P17" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="Q17" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="R17" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="S17" t="s">
-        <v>157</v>
+        <v>181</v>
       </c>
       <c r="T17">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="U17" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W17" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" spans="1:23">
       <c r="A18" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D18" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E18" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F18" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G18">
         <v>48</v>
@@ -2042,57 +2096,57 @@
         <v>2146</v>
       </c>
       <c r="L18" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M18" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N18" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O18" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P18" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="Q18" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="R18" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="S18" t="s">
-        <v>167</v>
+        <v>182</v>
       </c>
       <c r="T18">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="U18" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W18" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="19" spans="1:23">
       <c r="A19" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D19" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E19" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F19" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G19">
         <v>48</v>
@@ -2104,57 +2158,57 @@
         <v>2146</v>
       </c>
       <c r="L19" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M19" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N19" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O19" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P19" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="Q19" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="R19" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="S19" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="T19">
         <v>31</v>
       </c>
       <c r="U19" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W19" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:23">
       <c r="A20" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D20" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E20" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F20" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G20">
         <v>48</v>
@@ -2166,57 +2220,57 @@
         <v>2146</v>
       </c>
       <c r="L20" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M20" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N20" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O20" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P20" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="Q20" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="R20" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="S20" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="T20">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="U20" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W20" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21" spans="1:23">
       <c r="A21" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D21" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E21" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F21" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G21">
         <v>48</v>
@@ -2228,57 +2282,57 @@
         <v>2146</v>
       </c>
       <c r="L21" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M21" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N21" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O21" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P21" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="Q21" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="R21" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="S21" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="T21">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="U21" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W21" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22" spans="1:23">
       <c r="A22" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D22" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E22" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F22" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G22">
         <v>48</v>
@@ -2290,57 +2344,57 @@
         <v>2146</v>
       </c>
       <c r="L22" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M22" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N22" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O22" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P22" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="Q22" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="R22" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="S22" t="s">
-        <v>164</v>
+        <v>185</v>
       </c>
       <c r="T22">
         <v>30</v>
       </c>
       <c r="U22" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W22" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="23" spans="1:23">
       <c r="A23" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D23" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E23" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F23" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G23">
         <v>48</v>
@@ -2352,57 +2406,57 @@
         <v>2146</v>
       </c>
       <c r="L23" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M23" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N23" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O23" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P23" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="Q23" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="R23" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="S23" t="s">
-        <v>171</v>
+        <v>186</v>
       </c>
       <c r="T23">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="U23" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W23" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="24" spans="1:23">
       <c r="A24" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D24" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E24" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F24" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G24">
         <v>48</v>
@@ -2414,57 +2468,57 @@
         <v>2146</v>
       </c>
       <c r="L24" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M24" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N24" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O24" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P24" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="Q24" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="R24" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="S24" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="T24">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="U24" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W24" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="25" spans="1:23">
       <c r="A25" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D25" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E25" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F25" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G25">
         <v>48</v>
@@ -2476,57 +2530,57 @@
         <v>2146</v>
       </c>
       <c r="L25" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M25" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N25" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O25" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P25" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="Q25" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="R25" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="S25" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="T25">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="U25" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W25" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="26" spans="1:23">
       <c r="A26" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E26" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F26" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G26">
         <v>48</v>
@@ -2538,57 +2592,57 @@
         <v>2146</v>
       </c>
       <c r="L26" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M26" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N26" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O26" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P26" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="Q26" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="R26" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="S26" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="T26">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="U26" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W26" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="27" spans="1:23">
       <c r="A27" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D27" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E27" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F27" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G27">
         <v>48</v>
@@ -2600,57 +2654,57 @@
         <v>2146</v>
       </c>
       <c r="L27" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M27" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N27" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O27" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P27" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="Q27" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="R27" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="S27" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="T27">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="U27" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W27" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="28" spans="1:23">
       <c r="A28" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D28" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E28" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F28" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G28">
         <v>48</v>
@@ -2662,57 +2716,57 @@
         <v>2146</v>
       </c>
       <c r="L28" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M28" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N28" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O28" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P28" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="Q28" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="R28" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="S28" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="T28">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="U28" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W28" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="29" spans="1:23">
       <c r="A29" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B29" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D29" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E29" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F29" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G29">
         <v>48</v>
@@ -2724,57 +2778,57 @@
         <v>2146</v>
       </c>
       <c r="L29" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M29" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N29" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O29" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P29" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="Q29" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="R29" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="S29" t="s">
-        <v>162</v>
+        <v>191</v>
       </c>
       <c r="T29">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="U29" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W29" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="30" spans="1:23">
       <c r="A30" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C30" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D30" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E30" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F30" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G30">
         <v>48</v>
@@ -2786,57 +2840,57 @@
         <v>2146</v>
       </c>
       <c r="L30" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M30" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N30" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O30" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P30" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="Q30" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="R30" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="S30" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
       <c r="T30">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="U30" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W30" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="31" spans="1:23">
       <c r="A31" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C31" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D31" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E31" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F31" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G31">
         <v>48</v>
@@ -2848,57 +2902,57 @@
         <v>2146</v>
       </c>
       <c r="L31" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M31" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N31" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O31" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P31" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="Q31" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="R31" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="S31" t="s">
         <v>178</v>
       </c>
       <c r="T31">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="U31" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W31" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:23">
       <c r="A32" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B32" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C32" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D32" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E32" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F32" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G32">
         <v>48</v>
@@ -2910,57 +2964,57 @@
         <v>2146</v>
       </c>
       <c r="L32" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M32" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N32" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O32" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P32" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="Q32" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="R32" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="S32" t="s">
-        <v>161</v>
+        <v>193</v>
       </c>
       <c r="T32">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="U32" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W32" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="33" spans="1:23">
       <c r="A33" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B33" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C33" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D33" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E33" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F33" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G33">
         <v>48</v>
@@ -2972,57 +3026,57 @@
         <v>2146</v>
       </c>
       <c r="L33" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M33" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N33" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O33" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P33" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="Q33" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="R33" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
       <c r="S33" t="s">
-        <v>179</v>
+        <v>194</v>
       </c>
       <c r="T33">
         <v>25</v>
       </c>
       <c r="U33" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W33" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="34" spans="1:23">
       <c r="A34" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B34" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C34" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D34" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E34" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F34" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G34">
         <v>48</v>
@@ -3034,57 +3088,57 @@
         <v>2146</v>
       </c>
       <c r="L34" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M34" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N34" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O34" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P34" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="Q34" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="R34" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="S34" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="T34">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="U34" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W34" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="35" spans="1:23">
       <c r="A35" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B35" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C35" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D35" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E35" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F35" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G35">
         <v>48</v>
@@ -3096,57 +3150,57 @@
         <v>2146</v>
       </c>
       <c r="L35" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M35" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N35" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O35" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P35" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="Q35" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="R35" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="S35" t="s">
-        <v>168</v>
+        <v>195</v>
       </c>
       <c r="T35">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="U35" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W35" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="36" spans="1:23">
       <c r="A36" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B36" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C36" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D36" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E36" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F36" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G36">
         <v>48</v>
@@ -3158,57 +3212,57 @@
         <v>2146</v>
       </c>
       <c r="L36" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M36" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N36" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O36" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P36" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="Q36" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="R36" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="S36" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="T36">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="U36" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W36" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="37" spans="1:23">
       <c r="A37" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B37" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C37" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D37" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E37" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F37" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G37">
         <v>48</v>
@@ -3220,57 +3274,57 @@
         <v>2146</v>
       </c>
       <c r="L37" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M37" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N37" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O37" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P37" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="Q37" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="R37" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="S37" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="T37">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="U37" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W37" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="38" spans="1:23">
       <c r="A38" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B38" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C38" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D38" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E38" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F38" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G38">
         <v>48</v>
@@ -3282,57 +3336,57 @@
         <v>2146</v>
       </c>
       <c r="L38" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M38" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N38" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O38" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P38" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="Q38" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="R38" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="S38" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
       <c r="T38">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="U38" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W38" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="39" spans="1:23">
       <c r="A39" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B39" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C39" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D39" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E39" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F39" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G39">
         <v>48</v>
@@ -3344,57 +3398,57 @@
         <v>2146</v>
       </c>
       <c r="L39" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M39" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N39" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O39" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P39" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="Q39" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="R39" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="S39" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="T39">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="U39" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W39" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="40" spans="1:23">
       <c r="A40" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B40" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C40" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D40" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E40" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F40" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G40">
         <v>48</v>
@@ -3406,57 +3460,57 @@
         <v>2146</v>
       </c>
       <c r="L40" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M40" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N40" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O40" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P40" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="Q40" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="R40" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
       <c r="S40" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="T40">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="U40" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W40" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="41" spans="1:23">
       <c r="A41" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B41" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C41" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D41" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E41" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F41" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G41">
         <v>48</v>
@@ -3468,57 +3522,57 @@
         <v>2146</v>
       </c>
       <c r="L41" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M41" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N41" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O41" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P41" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="Q41" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="R41" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="S41" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
       <c r="T41">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="U41" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W41" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="42" spans="1:23">
       <c r="A42" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B42" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C42" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D42" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E42" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F42" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G42">
         <v>48</v>
@@ -3530,57 +3584,57 @@
         <v>2146</v>
       </c>
       <c r="L42" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M42" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N42" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O42" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P42" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="Q42" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="R42" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="S42" t="s">
-        <v>187</v>
+        <v>201</v>
       </c>
       <c r="T42">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="U42" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W42" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="43" spans="1:23">
       <c r="A43" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B43" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C43" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D43" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E43" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F43" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G43">
         <v>48</v>
@@ -3592,57 +3646,57 @@
         <v>2146</v>
       </c>
       <c r="L43" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M43" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N43" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O43" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P43" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="Q43" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="R43" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="S43" t="s">
-        <v>188</v>
+        <v>202</v>
       </c>
       <c r="T43">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="U43" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W43" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="44" spans="1:23">
       <c r="A44" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B44" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C44" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D44" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E44" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F44" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G44">
         <v>48</v>
@@ -3654,57 +3708,57 @@
         <v>2146</v>
       </c>
       <c r="L44" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M44" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N44" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O44" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P44" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="Q44" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="R44" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="S44" t="s">
-        <v>189</v>
+        <v>203</v>
       </c>
       <c r="T44">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="U44" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W44" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="45" spans="1:23">
       <c r="A45" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B45" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C45" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D45" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E45" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F45" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G45">
         <v>48</v>
@@ -3716,57 +3770,57 @@
         <v>2146</v>
       </c>
       <c r="L45" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M45" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N45" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O45" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P45" t="s">
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="Q45" t="s">
-        <v>84</v>
+        <v>119</v>
       </c>
       <c r="R45" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="S45" t="s">
-        <v>155</v>
+        <v>204</v>
       </c>
       <c r="T45">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="U45" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W45" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="46" spans="1:23">
       <c r="A46" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B46" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C46" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D46" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E46" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F46" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G46">
         <v>48</v>
@@ -3778,57 +3832,57 @@
         <v>2146</v>
       </c>
       <c r="L46" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M46" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N46" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O46" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P46" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="Q46" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="R46" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="S46" t="s">
-        <v>190</v>
+        <v>205</v>
       </c>
       <c r="T46">
-        <v>82</v>
+        <v>7</v>
       </c>
       <c r="U46" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W46" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="47" spans="1:23">
       <c r="A47" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B47" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C47" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D47" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E47" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F47" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G47">
         <v>48</v>
@@ -3840,37 +3894,161 @@
         <v>2146</v>
       </c>
       <c r="L47" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="M47" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N47" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="O47" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="P47" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="Q47" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="R47" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="S47" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="T47">
         <v>28</v>
       </c>
       <c r="U47" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="W47" t="s">
-        <v>22</v>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23">
+      <c r="A48" t="s">
+        <v>23</v>
+      </c>
+      <c r="B48" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" t="s">
+        <v>25</v>
+      </c>
+      <c r="D48" t="s">
+        <v>26</v>
+      </c>
+      <c r="E48" t="s">
+        <v>27</v>
+      </c>
+      <c r="F48" t="s">
+        <v>28</v>
+      </c>
+      <c r="G48">
+        <v>48</v>
+      </c>
+      <c r="H48">
+        <v>115</v>
+      </c>
+      <c r="I48">
+        <v>2146</v>
+      </c>
+      <c r="L48" t="s">
+        <v>29</v>
+      </c>
+      <c r="M48" t="s">
+        <v>30</v>
+      </c>
+      <c r="N48" t="s">
+        <v>30</v>
+      </c>
+      <c r="O48" t="s">
+        <v>31</v>
+      </c>
+      <c r="P48" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>120</v>
+      </c>
+      <c r="R48" t="s">
+        <v>166</v>
+      </c>
+      <c r="S48" t="s">
+        <v>206</v>
+      </c>
+      <c r="T48">
+        <v>82</v>
+      </c>
+      <c r="U48" t="s">
+        <v>208</v>
+      </c>
+      <c r="W48" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23">
+      <c r="A49" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49" t="s">
+        <v>24</v>
+      </c>
+      <c r="C49" t="s">
+        <v>25</v>
+      </c>
+      <c r="D49" t="s">
+        <v>26</v>
+      </c>
+      <c r="E49" t="s">
+        <v>27</v>
+      </c>
+      <c r="F49" t="s">
+        <v>28</v>
+      </c>
+      <c r="G49">
+        <v>48</v>
+      </c>
+      <c r="H49">
+        <v>115</v>
+      </c>
+      <c r="I49">
+        <v>2146</v>
+      </c>
+      <c r="L49" t="s">
+        <v>29</v>
+      </c>
+      <c r="M49" t="s">
+        <v>30</v>
+      </c>
+      <c r="N49" t="s">
+        <v>30</v>
+      </c>
+      <c r="O49" t="s">
+        <v>31</v>
+      </c>
+      <c r="P49" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>121</v>
+      </c>
+      <c r="R49" t="s">
+        <v>167</v>
+      </c>
+      <c r="S49" t="s">
+        <v>184</v>
+      </c>
+      <c r="T49">
+        <v>28</v>
+      </c>
+      <c r="U49" t="s">
+        <v>208</v>
+      </c>
+      <c r="W49" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>